<commit_message>
k you can do this
</commit_message>
<xml_diff>
--- a/Lab4/lab4.xlsx
+++ b/Lab4/lab4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aruns\Documents\Stat 235\Labs\Stat-235-Labs\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EE3513-4E39-4183-A38F-439892481F29}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C07D22A-130B-4161-95CD-05F95A2C29A2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16865,7 +16865,7 @@
   <dimension ref="A1:CZ49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B49" sqref="A36:B49"/>
+      <selection activeCell="H49" sqref="G36:H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
I guess I missed this bit for part 4
</commit_message>
<xml_diff>
--- a/Lab4/lab4.xlsx
+++ b/Lab4/lab4.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aruns\Documents\Stat 235\Labs\Stat-235-Labs\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C07D22A-130B-4161-95CD-05F95A2C29A2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866CA538-0666-4BF1-A03C-E74607BE8EE4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation" sheetId="4" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
   <si>
     <t>Sample mean</t>
   </si>
@@ -121,6 +122,57 @@
   </si>
   <si>
     <t>Confidence Level(95.0%)</t>
+  </si>
+  <si>
+    <t>#rejected</t>
+  </si>
+  <si>
+    <t>fraction</t>
+  </si>
+  <si>
+    <t>t-Test: Two-Sample Assuming Unequal Variances</t>
+  </si>
+  <si>
+    <t>Variable 1</t>
+  </si>
+  <si>
+    <t>Variable 2</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Hypothesized Mean Difference</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) one-tail</t>
+  </si>
+  <si>
+    <t>t Critical one-tail</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) two-tail</t>
+  </si>
+  <si>
+    <t>t Critical two-tail</t>
+  </si>
+  <si>
+    <t>t-Test: Paired Two Sample for Means</t>
+  </si>
+  <si>
+    <t>Pearson Correlation</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -339,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -398,6 +450,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -414,6 +469,1105 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Effect vs Alloy 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>64.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>66.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>65.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>65.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>64.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>64.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>65.3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>67.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>64.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>65.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>64.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>66.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>64.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>64.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.7999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0999999999999943</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9000000000000057</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2000000000000028</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1999999999999886</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4000000000000057</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.9999999999994316E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.89999999999999147</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6000000000000085</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8000000000000114</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0999999999999943</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.2000000000000028</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.5999999999999943</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.2999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.69999999999998863</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.9000000000000057</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.8000000000000114</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.9000000000000057</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.80000000000001137</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.5999999999999943</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.8999999999999915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E887-414E-82A9-C96781377A97}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1258945855"/>
+        <c:axId val="981285279"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1258945855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981285279"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="981285279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1258945855"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>206375</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>17463</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>500063</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>141288</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEDCD58F-FB7A-495B-A065-2AECD2B3267C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -716,7 +1870,7 @@
   <dimension ref="A1:CY78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -730,7 +1884,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="13">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="D1" s="19">
         <v>62.723180851811776</v>
@@ -1654,7 +2808,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="D4" s="19">
         <v>63.579713403363712</v>
@@ -10220,403 +11374,403 @@
       </c>
       <c r="D32" s="7">
         <f>CONFIDENCE(1-$B$1,$B$2, 30)</f>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="E32" s="8">
         <f t="shared" ref="E32:BP32" si="2">CONFIDENCE(1-$B$1,$B$2, 30)</f>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="F32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="G32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="H32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="I32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="J32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="K32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="L32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="M32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="N32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="O32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="P32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="Q32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="R32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="S32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="T32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="U32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="V32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="W32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="X32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="Y32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="Z32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AA32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AB32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AC32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AD32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AE32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AF32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AG32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AH32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AI32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AJ32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AK32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AL32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AM32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AN32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AO32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AP32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AQ32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AR32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AS32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AT32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AU32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AV32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AW32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AX32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AY32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="AZ32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BA32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BB32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BC32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BD32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BE32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BF32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BG32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BH32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BI32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BJ32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BK32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BL32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BM32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BN32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BO32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BP32" s="8">
         <f t="shared" si="2"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BQ32" s="8">
         <f t="shared" ref="BQ32:CY32" si="3">CONFIDENCE(1-$B$1,$B$2, 30)</f>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BR32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BS32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BT32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BU32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BV32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BW32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BX32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BY32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="BZ32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CA32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CB32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CC32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CD32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CE32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CF32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CG32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CH32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CI32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CJ32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CK32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CL32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CM32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CN32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CO32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CP32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CQ32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CR32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CS32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CT32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CU32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CV32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CW32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CX32" s="8">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
       <c r="CY32" s="9">
         <f t="shared" si="3"/>
-        <v>0.35783882874343131</v>
+        <v>0.3003078117585028</v>
       </c>
     </row>
     <row r="33" spans="1:103" x14ac:dyDescent="0.2">
@@ -10625,403 +11779,403 @@
       </c>
       <c r="D33" s="7">
         <f>D31-D32</f>
-        <v>63.867589096472194</v>
+        <v>63.925120113457126</v>
       </c>
       <c r="E33" s="8">
         <f t="shared" ref="E33:BP33" si="4">E31-E32</f>
-        <v>63.685680795901298</v>
+        <v>63.74321181288623</v>
       </c>
       <c r="F33" s="8">
         <f t="shared" si="4"/>
-        <v>63.482507751290711</v>
+        <v>63.540038768275643</v>
       </c>
       <c r="G33" s="8">
         <f t="shared" si="4"/>
-        <v>63.637675581283034</v>
+        <v>63.695206598267966</v>
       </c>
       <c r="H33" s="8">
         <f t="shared" si="4"/>
-        <v>63.468382389077476</v>
+        <v>63.525913406062408</v>
       </c>
       <c r="I33" s="8">
         <f t="shared" si="4"/>
-        <v>63.919881593323389</v>
+        <v>63.97741261030832</v>
       </c>
       <c r="J33" s="8">
         <f t="shared" si="4"/>
-        <v>63.58786858186933</v>
+        <v>63.645399598854262</v>
       </c>
       <c r="K33" s="8">
         <f t="shared" si="4"/>
-        <v>63.746859321258107</v>
+        <v>63.804390338243039</v>
       </c>
       <c r="L33" s="8">
         <f t="shared" si="4"/>
-        <v>63.647906941930636</v>
+        <v>63.705437958915567</v>
       </c>
       <c r="M33" s="8">
         <f t="shared" si="4"/>
-        <v>63.763403825691221</v>
+        <v>63.820934842676152</v>
       </c>
       <c r="N33" s="8">
         <f t="shared" si="4"/>
-        <v>63.311591489998605</v>
+        <v>63.369122506983537</v>
       </c>
       <c r="O33" s="8">
         <f t="shared" si="4"/>
-        <v>63.580388897441949</v>
+        <v>63.637919914426881</v>
       </c>
       <c r="P33" s="8">
         <f t="shared" si="4"/>
-        <v>63.760201002203324</v>
+        <v>63.817732019188256</v>
       </c>
       <c r="Q33" s="8">
         <f t="shared" si="4"/>
-        <v>63.745160385155195</v>
+        <v>63.802691402140127</v>
       </c>
       <c r="R33" s="8">
         <f t="shared" si="4"/>
-        <v>64.072067834414028</v>
+        <v>64.129598851398953</v>
       </c>
       <c r="S33" s="8">
         <f t="shared" si="4"/>
-        <v>63.425907698053848</v>
+        <v>63.48343871503878</v>
       </c>
       <c r="T33" s="8">
         <f t="shared" si="4"/>
-        <v>63.593004195285346</v>
+        <v>63.650535212270277</v>
       </c>
       <c r="U33" s="8">
         <f t="shared" si="4"/>
-        <v>63.957754695903397</v>
+        <v>64.015285712888328</v>
       </c>
       <c r="V33" s="8">
         <f t="shared" si="4"/>
-        <v>63.243184149169657</v>
+        <v>63.300715166154589</v>
       </c>
       <c r="W33" s="8">
         <f t="shared" si="4"/>
-        <v>63.480195019950941</v>
+        <v>63.537726036935872</v>
       </c>
       <c r="X33" s="8">
         <f t="shared" si="4"/>
-        <v>63.824981619222108</v>
+        <v>63.882512636207039</v>
       </c>
       <c r="Y33" s="8">
         <f t="shared" si="4"/>
-        <v>63.646743167668482</v>
+        <v>63.704274184653414</v>
       </c>
       <c r="Z33" s="8">
         <f t="shared" si="4"/>
-        <v>63.821205131951068</v>
+        <v>63.878736148935999</v>
       </c>
       <c r="AA33" s="8">
         <f t="shared" si="4"/>
-        <v>63.659236176370108</v>
+        <v>63.716767193355039</v>
       </c>
       <c r="AB33" s="8">
         <f t="shared" si="4"/>
-        <v>63.743696932388822</v>
+        <v>63.801227949373754</v>
       </c>
       <c r="AC33" s="8">
         <f t="shared" si="4"/>
-        <v>63.827700477841837</v>
+        <v>63.885231494826769</v>
       </c>
       <c r="AD33" s="8">
         <f t="shared" si="4"/>
-        <v>63.284031526798131</v>
+        <v>63.341562543783063</v>
       </c>
       <c r="AE33" s="8">
         <f t="shared" si="4"/>
-        <v>63.654563154696781</v>
+        <v>63.712094171681713</v>
       </c>
       <c r="AF33" s="8">
         <f t="shared" si="4"/>
-        <v>63.546661347503857</v>
+        <v>63.604192364488789</v>
       </c>
       <c r="AG33" s="8">
         <f t="shared" si="4"/>
-        <v>63.080760711507097</v>
+        <v>63.138291728492028</v>
       </c>
       <c r="AH33" s="8">
         <f t="shared" si="4"/>
-        <v>63.793538947348544</v>
+        <v>63.851069964333476</v>
       </c>
       <c r="AI33" s="8">
         <f t="shared" si="4"/>
-        <v>63.566079627820898</v>
+        <v>63.623610644805829</v>
       </c>
       <c r="AJ33" s="8">
         <f t="shared" si="4"/>
-        <v>63.297231364465475</v>
+        <v>63.354762381450406</v>
       </c>
       <c r="AK33" s="8">
         <f t="shared" si="4"/>
-        <v>63.814432958610432</v>
+        <v>63.871963975595364</v>
       </c>
       <c r="AL33" s="8">
         <f t="shared" si="4"/>
-        <v>63.677087738376507</v>
+        <v>63.734618755361439</v>
       </c>
       <c r="AM33" s="8">
         <f t="shared" si="4"/>
-        <v>63.613332159782217</v>
+        <v>63.670863176767149</v>
       </c>
       <c r="AN33" s="8">
         <f t="shared" si="4"/>
-        <v>63.666372450756334</v>
+        <v>63.723903467741266</v>
       </c>
       <c r="AO33" s="8">
         <f t="shared" si="4"/>
-        <v>63.829917522759864</v>
+        <v>63.887448539744796</v>
       </c>
       <c r="AP33" s="8">
         <f t="shared" si="4"/>
-        <v>63.672036442698463</v>
+        <v>63.729567459683395</v>
       </c>
       <c r="AQ33" s="8">
         <f t="shared" si="4"/>
-        <v>63.823021279183671</v>
+        <v>63.880552296168602</v>
       </c>
       <c r="AR33" s="8">
         <f t="shared" si="4"/>
-        <v>63.763265809870227</v>
+        <v>63.820796826855158</v>
       </c>
       <c r="AS33" s="8">
         <f t="shared" si="4"/>
-        <v>63.483220491971998</v>
+        <v>63.54075150895693</v>
       </c>
       <c r="AT33" s="8">
         <f t="shared" si="4"/>
-        <v>63.832232035193421</v>
+        <v>63.889763052178353</v>
       </c>
       <c r="AU33" s="8">
         <f t="shared" si="4"/>
-        <v>63.639263672719167</v>
+        <v>63.696794689704099</v>
       </c>
       <c r="AV33" s="8">
         <f t="shared" si="4"/>
-        <v>63.763301242267993</v>
+        <v>63.820832259252924</v>
       </c>
       <c r="AW33" s="8">
         <f t="shared" si="4"/>
-        <v>63.344984307990842</v>
+        <v>63.402515324975774</v>
       </c>
       <c r="AX33" s="8">
         <f t="shared" si="4"/>
-        <v>63.699062115657263</v>
+        <v>63.756593132642195</v>
       </c>
       <c r="AY33" s="8">
         <f t="shared" si="4"/>
-        <v>63.347284799047749</v>
+        <v>63.404815816032681</v>
       </c>
       <c r="AZ33" s="8">
         <f t="shared" si="4"/>
-        <v>63.782661049654827</v>
+        <v>63.840192066639759</v>
       </c>
       <c r="BA33" s="8">
         <f t="shared" si="4"/>
-        <v>63.672622953094269</v>
+        <v>63.730153970079201</v>
       </c>
       <c r="BB33" s="8">
         <f t="shared" si="4"/>
-        <v>63.493111891079195</v>
+        <v>63.550642908064127</v>
       </c>
       <c r="BC33" s="8">
         <f t="shared" si="4"/>
-        <v>63.7950140719636</v>
+        <v>63.852545088948531</v>
       </c>
       <c r="BD33" s="8">
         <f t="shared" si="4"/>
-        <v>63.765181281503395</v>
+        <v>63.822712298488327</v>
       </c>
       <c r="BE33" s="8">
         <f t="shared" si="4"/>
-        <v>63.338989676829001</v>
+        <v>63.396520693813933</v>
       </c>
       <c r="BF33" s="8">
         <f t="shared" si="4"/>
-        <v>63.673313183781694</v>
+        <v>63.730844200766626</v>
       </c>
       <c r="BG33" s="8">
         <f t="shared" si="4"/>
-        <v>63.557222134711552</v>
+        <v>63.614753151696483</v>
       </c>
       <c r="BH33" s="8">
         <f t="shared" si="4"/>
-        <v>63.757026031990655</v>
+        <v>63.814557048975587</v>
       </c>
       <c r="BI33" s="8">
         <f t="shared" si="4"/>
-        <v>63.827096838629153</v>
+        <v>63.884627855614085</v>
       </c>
       <c r="BJ33" s="8">
         <f t="shared" si="4"/>
-        <v>63.090442093129411</v>
+        <v>63.147973110114343</v>
       </c>
       <c r="BK33" s="8">
         <f t="shared" si="4"/>
-        <v>63.528490173901005</v>
+        <v>63.586021190885937</v>
       </c>
       <c r="BL33" s="8">
         <f t="shared" si="4"/>
-        <v>63.682910853995828</v>
+        <v>63.74044187098076</v>
       </c>
       <c r="BM33" s="8">
         <f t="shared" si="4"/>
-        <v>63.631648018833872</v>
+        <v>63.689179035818803</v>
       </c>
       <c r="BN33" s="8">
         <f t="shared" si="4"/>
-        <v>63.359119485167732</v>
+        <v>63.416650502152663</v>
       </c>
       <c r="BO33" s="8">
         <f t="shared" si="4"/>
-        <v>63.823318418681858</v>
+        <v>63.880849435666789</v>
       </c>
       <c r="BP33" s="8">
         <f t="shared" si="4"/>
-        <v>63.620579733582588</v>
+        <v>63.678110750567519</v>
       </c>
       <c r="BQ33" s="8">
         <f t="shared" ref="BQ33:CY33" si="5">BQ31-BQ32</f>
-        <v>63.698817992121057</v>
+        <v>63.756349009105989</v>
       </c>
       <c r="BR33" s="8">
         <f t="shared" si="5"/>
-        <v>63.62090150522895</v>
+        <v>63.678432522213882</v>
       </c>
       <c r="BS33" s="8">
         <f t="shared" si="5"/>
-        <v>63.497404099741757</v>
+        <v>63.554935116726689</v>
       </c>
       <c r="BT33" s="8">
         <f t="shared" si="5"/>
-        <v>63.321433624809458</v>
+        <v>63.37896464179439</v>
       </c>
       <c r="BU33" s="8">
         <f t="shared" si="5"/>
-        <v>63.937691887007695</v>
+        <v>63.995222903992627</v>
       </c>
       <c r="BV33" s="8">
         <f t="shared" si="5"/>
-        <v>63.885193124337256</v>
+        <v>63.942724141322188</v>
       </c>
       <c r="BW33" s="8">
         <f t="shared" si="5"/>
-        <v>63.93529893065611</v>
+        <v>63.992829947641042</v>
       </c>
       <c r="BX33" s="8">
         <f t="shared" si="5"/>
-        <v>63.360827629904499</v>
+        <v>63.41835864688943</v>
       </c>
       <c r="BY33" s="8">
         <f t="shared" si="5"/>
-        <v>63.422939031556041</v>
+        <v>63.480470048540973</v>
       </c>
       <c r="BZ33" s="8">
         <f t="shared" si="5"/>
-        <v>63.792040327453698</v>
+        <v>63.84957134443863</v>
       </c>
       <c r="CA33" s="8">
         <f t="shared" si="5"/>
-        <v>63.625019659342968</v>
+        <v>63.682550676327899</v>
       </c>
       <c r="CB33" s="8">
         <f t="shared" si="5"/>
-        <v>63.5167373801998</v>
+        <v>63.574268397184731</v>
       </c>
       <c r="CC33" s="8">
         <f t="shared" si="5"/>
-        <v>63.569445629816542</v>
+        <v>63.626976646801474</v>
       </c>
       <c r="CD33" s="8">
         <f t="shared" si="5"/>
-        <v>63.505667617019618</v>
+        <v>63.56319863400455</v>
       </c>
       <c r="CE33" s="8">
         <f t="shared" si="5"/>
-        <v>63.70124588822744</v>
+        <v>63.758776905212372</v>
       </c>
       <c r="CF33" s="8">
         <f t="shared" si="5"/>
-        <v>63.595292711328682</v>
+        <v>63.652823728313614</v>
       </c>
       <c r="CG33" s="8">
         <f t="shared" si="5"/>
-        <v>63.654392851813874</v>
+        <v>63.711923868798806</v>
       </c>
       <c r="CH33" s="8">
         <f t="shared" si="5"/>
-        <v>63.651364916577997</v>
+        <v>63.708895933562928</v>
       </c>
       <c r="CI33" s="8">
         <f t="shared" si="5"/>
-        <v>63.681372102647266</v>
+        <v>63.738903119632198</v>
       </c>
       <c r="CJ33" s="8">
         <f t="shared" si="5"/>
-        <v>63.268755805369608</v>
+        <v>63.32628682235454</v>
       </c>
       <c r="CK33" s="8">
         <f t="shared" si="5"/>
-        <v>63.563296346659797</v>
+        <v>63.620827363644729</v>
       </c>
       <c r="CL33" s="8">
         <f t="shared" si="5"/>
-        <v>63.3808286689517</v>
+        <v>63.438359685936632</v>
       </c>
       <c r="CM33" s="8">
         <f t="shared" si="5"/>
-        <v>63.623246144674511</v>
+        <v>63.680777161659442</v>
       </c>
       <c r="CN33" s="8">
         <f t="shared" si="5"/>
-        <v>63.689574949049394</v>
+        <v>63.747105966034326</v>
       </c>
       <c r="CO33" s="8">
         <f t="shared" si="5"/>
-        <v>63.421792954544969</v>
+        <v>63.479323971529901</v>
       </c>
       <c r="CP33" s="8">
         <f t="shared" si="5"/>
-        <v>63.477530465744032</v>
+        <v>63.535061482728963</v>
       </c>
       <c r="CQ33" s="8">
         <f t="shared" si="5"/>
-        <v>63.381116448233584</v>
+        <v>63.438647465218516</v>
       </c>
       <c r="CR33" s="8">
         <f t="shared" si="5"/>
-        <v>63.63489548335339</v>
+        <v>63.692426500338321</v>
       </c>
       <c r="CS33" s="8">
         <f t="shared" si="5"/>
-        <v>63.691563672901658</v>
+        <v>63.74909468988659</v>
       </c>
       <c r="CT33" s="8">
         <f t="shared" si="5"/>
-        <v>63.666375141344837</v>
+        <v>63.723906158329768</v>
       </c>
       <c r="CU33" s="8">
         <f t="shared" si="5"/>
-        <v>63.935830113457563</v>
+        <v>63.993361130442494</v>
       </c>
       <c r="CV33" s="8">
         <f t="shared" si="5"/>
-        <v>63.375078502386579</v>
+        <v>63.43260951937151</v>
       </c>
       <c r="CW33" s="8">
         <f t="shared" si="5"/>
-        <v>63.698273015316637</v>
+        <v>63.755804032301569</v>
       </c>
       <c r="CX33" s="8">
         <f t="shared" si="5"/>
-        <v>63.885548585183209</v>
+        <v>63.94307960216814</v>
       </c>
       <c r="CY33" s="9">
         <f t="shared" si="5"/>
-        <v>63.842479311998297</v>
+        <v>63.900010328983228</v>
       </c>
     </row>
     <row r="34" spans="1:103" x14ac:dyDescent="0.2">
@@ -11030,403 +12184,403 @@
       </c>
       <c r="D34" s="7">
         <f>D31+D32</f>
-        <v>64.583266753959052</v>
+        <v>64.525735736974127</v>
       </c>
       <c r="E34" s="8">
         <f t="shared" ref="E34:BP34" si="6">E31+E32</f>
-        <v>64.401358453388156</v>
+        <v>64.343827436403231</v>
       </c>
       <c r="F34" s="8">
         <f t="shared" si="6"/>
-        <v>64.198185408777576</v>
+        <v>64.140654391792651</v>
       </c>
       <c r="G34" s="8">
         <f t="shared" si="6"/>
-        <v>64.353353238769898</v>
+        <v>64.295822221784974</v>
       </c>
       <c r="H34" s="8">
         <f t="shared" si="6"/>
-        <v>64.18406004656434</v>
+        <v>64.126529029579416</v>
       </c>
       <c r="I34" s="8">
         <f t="shared" si="6"/>
-        <v>64.635559250810246</v>
+        <v>64.578028233825322</v>
       </c>
       <c r="J34" s="8">
         <f t="shared" si="6"/>
-        <v>64.303546239356194</v>
+        <v>64.24601522237127</v>
       </c>
       <c r="K34" s="8">
         <f t="shared" si="6"/>
-        <v>64.462536978744964</v>
+        <v>64.40500596176004</v>
       </c>
       <c r="L34" s="8">
         <f t="shared" si="6"/>
-        <v>64.363584599417493</v>
+        <v>64.306053582432568</v>
       </c>
       <c r="M34" s="8">
         <f t="shared" si="6"/>
-        <v>64.479081483178078</v>
+        <v>64.421550466193153</v>
       </c>
       <c r="N34" s="8">
         <f t="shared" si="6"/>
-        <v>64.02726914748547</v>
+        <v>63.969738130500538</v>
       </c>
       <c r="O34" s="8">
         <f t="shared" si="6"/>
-        <v>64.296066554928814</v>
+        <v>64.238535537943889</v>
       </c>
       <c r="P34" s="8">
         <f t="shared" si="6"/>
-        <v>64.475878659690181</v>
+        <v>64.418347642705257</v>
       </c>
       <c r="Q34" s="8">
         <f t="shared" si="6"/>
-        <v>64.460838042642052</v>
+        <v>64.403307025657128</v>
       </c>
       <c r="R34" s="8">
         <f t="shared" si="6"/>
-        <v>64.787745491900878</v>
+        <v>64.730214474915954</v>
       </c>
       <c r="S34" s="8">
         <f t="shared" si="6"/>
-        <v>64.141585355540712</v>
+        <v>64.084054338555788</v>
       </c>
       <c r="T34" s="8">
         <f t="shared" si="6"/>
-        <v>64.30868185277221</v>
+        <v>64.251150835787286</v>
       </c>
       <c r="U34" s="8">
         <f t="shared" si="6"/>
-        <v>64.673432353390254</v>
+        <v>64.615901336405329</v>
       </c>
       <c r="V34" s="8">
         <f t="shared" si="6"/>
-        <v>63.958861806656522</v>
+        <v>63.90133078967159</v>
       </c>
       <c r="W34" s="8">
         <f t="shared" si="6"/>
-        <v>64.195872677437805</v>
+        <v>64.13834166045288</v>
       </c>
       <c r="X34" s="8">
         <f t="shared" si="6"/>
-        <v>64.540659276708965</v>
+        <v>64.48312825972404</v>
       </c>
       <c r="Y34" s="8">
         <f t="shared" si="6"/>
-        <v>64.36242082515534</v>
+        <v>64.304889808170415</v>
       </c>
       <c r="Z34" s="8">
         <f t="shared" si="6"/>
-        <v>64.536882789437925</v>
+        <v>64.479351772453001</v>
       </c>
       <c r="AA34" s="8">
         <f t="shared" si="6"/>
-        <v>64.374913833856965</v>
+        <v>64.317382816872041</v>
       </c>
       <c r="AB34" s="8">
         <f t="shared" si="6"/>
-        <v>64.459374589875679</v>
+        <v>64.401843572890755</v>
       </c>
       <c r="AC34" s="8">
         <f t="shared" si="6"/>
-        <v>64.543378135328695</v>
+        <v>64.48584711834377</v>
       </c>
       <c r="AD34" s="8">
         <f t="shared" si="6"/>
-        <v>63.999709184284995</v>
+        <v>63.942178167300064</v>
       </c>
       <c r="AE34" s="8">
         <f t="shared" si="6"/>
-        <v>64.370240812183638</v>
+        <v>64.312709795198714</v>
       </c>
       <c r="AF34" s="8">
         <f t="shared" si="6"/>
-        <v>64.262339004990721</v>
+        <v>64.204807988005797</v>
       </c>
       <c r="AG34" s="8">
         <f t="shared" si="6"/>
-        <v>63.796438368993961</v>
+        <v>63.738907352009029</v>
       </c>
       <c r="AH34" s="8">
         <f t="shared" si="6"/>
-        <v>64.509216604835402</v>
+        <v>64.451685587850477</v>
       </c>
       <c r="AI34" s="8">
         <f t="shared" si="6"/>
-        <v>64.281757285307762</v>
+        <v>64.224226268322838</v>
       </c>
       <c r="AJ34" s="8">
         <f t="shared" si="6"/>
-        <v>64.012909021952339</v>
+        <v>63.955378004967407</v>
       </c>
       <c r="AK34" s="8">
         <f t="shared" si="6"/>
-        <v>64.530110616097289</v>
+        <v>64.472579599112365</v>
       </c>
       <c r="AL34" s="8">
         <f t="shared" si="6"/>
-        <v>64.392765395863364</v>
+        <v>64.33523437887844</v>
       </c>
       <c r="AM34" s="8">
         <f t="shared" si="6"/>
-        <v>64.329009817269082</v>
+        <v>64.271478800284157</v>
       </c>
       <c r="AN34" s="8">
         <f t="shared" si="6"/>
-        <v>64.382050108243192</v>
+        <v>64.324519091258267</v>
       </c>
       <c r="AO34" s="8">
         <f t="shared" si="6"/>
-        <v>64.545595180246721</v>
+        <v>64.488064163261797</v>
       </c>
       <c r="AP34" s="8">
         <f t="shared" si="6"/>
-        <v>64.38771410018532</v>
+        <v>64.330183083200396</v>
       </c>
       <c r="AQ34" s="8">
         <f t="shared" si="6"/>
-        <v>64.538698936670528</v>
+        <v>64.481167919685603</v>
       </c>
       <c r="AR34" s="8">
         <f t="shared" si="6"/>
-        <v>64.478943467357084</v>
+        <v>64.421412450372159</v>
       </c>
       <c r="AS34" s="8">
         <f t="shared" si="6"/>
-        <v>64.198898149458856</v>
+        <v>64.141367132473931</v>
       </c>
       <c r="AT34" s="8">
         <f t="shared" si="6"/>
-        <v>64.547909692680278</v>
+        <v>64.490378675695354</v>
       </c>
       <c r="AU34" s="8">
         <f t="shared" si="6"/>
-        <v>64.354941330206032</v>
+        <v>64.297410313221107</v>
       </c>
       <c r="AV34" s="8">
         <f t="shared" si="6"/>
-        <v>64.47897889975485</v>
+        <v>64.421447882769925</v>
       </c>
       <c r="AW34" s="8">
         <f t="shared" si="6"/>
-        <v>64.060661965477706</v>
+        <v>64.003130948492782</v>
       </c>
       <c r="AX34" s="8">
         <f t="shared" si="6"/>
-        <v>64.41473977314412</v>
+        <v>64.357208756159196</v>
       </c>
       <c r="AY34" s="8">
         <f t="shared" si="6"/>
-        <v>64.062962456534606</v>
+        <v>64.005431439549682</v>
       </c>
       <c r="AZ34" s="8">
         <f t="shared" si="6"/>
-        <v>64.498338707141684</v>
+        <v>64.44080769015676</v>
       </c>
       <c r="BA34" s="8">
         <f t="shared" si="6"/>
-        <v>64.388300610581126</v>
+        <v>64.330769593596202</v>
       </c>
       <c r="BB34" s="8">
         <f t="shared" si="6"/>
-        <v>64.20878954856606</v>
+        <v>64.151258531581135</v>
       </c>
       <c r="BC34" s="8">
         <f t="shared" si="6"/>
-        <v>64.510691729450457</v>
+        <v>64.453160712465532</v>
       </c>
       <c r="BD34" s="8">
         <f t="shared" si="6"/>
-        <v>64.480858938990252</v>
+        <v>64.423327922005328</v>
       </c>
       <c r="BE34" s="8">
         <f t="shared" si="6"/>
-        <v>64.054667334315866</v>
+        <v>63.997136317330934</v>
       </c>
       <c r="BF34" s="8">
         <f t="shared" si="6"/>
-        <v>64.388990841268551</v>
+        <v>64.331459824283627</v>
       </c>
       <c r="BG34" s="8">
         <f t="shared" si="6"/>
-        <v>64.272899792198416</v>
+        <v>64.215368775213491</v>
       </c>
       <c r="BH34" s="8">
         <f t="shared" si="6"/>
-        <v>64.472703689477513</v>
+        <v>64.415172672492588</v>
       </c>
       <c r="BI34" s="8">
         <f t="shared" si="6"/>
-        <v>64.54277449611601</v>
+        <v>64.485243479131086</v>
       </c>
       <c r="BJ34" s="8">
         <f t="shared" si="6"/>
-        <v>63.806119750616276</v>
+        <v>63.748588733631344</v>
       </c>
       <c r="BK34" s="8">
         <f t="shared" si="6"/>
-        <v>64.24416783138787</v>
+        <v>64.186636814402945</v>
       </c>
       <c r="BL34" s="8">
         <f t="shared" si="6"/>
-        <v>64.398588511482686</v>
+        <v>64.341057494497761</v>
       </c>
       <c r="BM34" s="8">
         <f t="shared" si="6"/>
-        <v>64.347325676320736</v>
+        <v>64.289794659335811</v>
       </c>
       <c r="BN34" s="8">
         <f t="shared" si="6"/>
-        <v>64.074797142654589</v>
+        <v>64.017266125669664</v>
       </c>
       <c r="BO34" s="8">
         <f t="shared" si="6"/>
-        <v>64.538996076168715</v>
+        <v>64.48146505918379</v>
       </c>
       <c r="BP34" s="8">
         <f t="shared" si="6"/>
-        <v>64.336257391069452</v>
+        <v>64.278726374084528</v>
       </c>
       <c r="BQ34" s="8">
         <f t="shared" ref="BQ34:CY34" si="7">BQ31+BQ32</f>
-        <v>64.414495649607915</v>
+        <v>64.35696463262299</v>
       </c>
       <c r="BR34" s="8">
         <f t="shared" si="7"/>
-        <v>64.336579162715807</v>
+        <v>64.279048145730883</v>
       </c>
       <c r="BS34" s="8">
         <f t="shared" si="7"/>
-        <v>64.213081757228622</v>
+        <v>64.155550740243697</v>
       </c>
       <c r="BT34" s="8">
         <f t="shared" si="7"/>
-        <v>64.037111282296323</v>
+        <v>63.979580265311391</v>
       </c>
       <c r="BU34" s="8">
         <f t="shared" si="7"/>
-        <v>64.653369544494552</v>
+        <v>64.595838527509628</v>
       </c>
       <c r="BV34" s="8">
         <f t="shared" si="7"/>
-        <v>64.600870781824113</v>
+        <v>64.543339764839189</v>
       </c>
       <c r="BW34" s="8">
         <f t="shared" si="7"/>
-        <v>64.650976588142967</v>
+        <v>64.593445571158043</v>
       </c>
       <c r="BX34" s="8">
         <f t="shared" si="7"/>
-        <v>64.076505287391356</v>
+        <v>64.018974270406432</v>
       </c>
       <c r="BY34" s="8">
         <f t="shared" si="7"/>
-        <v>64.138616689042905</v>
+        <v>64.081085672057981</v>
       </c>
       <c r="BZ34" s="8">
         <f t="shared" si="7"/>
-        <v>64.507717984940555</v>
+        <v>64.450186967955631</v>
       </c>
       <c r="CA34" s="8">
         <f t="shared" si="7"/>
-        <v>64.340697316829832</v>
+        <v>64.283166299844908</v>
       </c>
       <c r="CB34" s="8">
         <f t="shared" si="7"/>
-        <v>64.232415037686664</v>
+        <v>64.174884020701739</v>
       </c>
       <c r="CC34" s="8">
         <f t="shared" si="7"/>
-        <v>64.285123287303406</v>
+        <v>64.227592270318482</v>
       </c>
       <c r="CD34" s="8">
         <f t="shared" si="7"/>
-        <v>64.221345274506476</v>
+        <v>64.163814257521551</v>
       </c>
       <c r="CE34" s="8">
         <f t="shared" si="7"/>
-        <v>64.416923545714297</v>
+        <v>64.359392528729373</v>
       </c>
       <c r="CF34" s="8">
         <f t="shared" si="7"/>
-        <v>64.310970368815546</v>
+        <v>64.253439351830622</v>
       </c>
       <c r="CG34" s="8">
         <f t="shared" si="7"/>
-        <v>64.370070509300731</v>
+        <v>64.312539492315807</v>
       </c>
       <c r="CH34" s="8">
         <f t="shared" si="7"/>
-        <v>64.367042574064854</v>
+        <v>64.309511557079929</v>
       </c>
       <c r="CI34" s="8">
         <f t="shared" si="7"/>
-        <v>64.397049760134124</v>
+        <v>64.339518743149199</v>
       </c>
       <c r="CJ34" s="8">
         <f t="shared" si="7"/>
-        <v>63.984433462856472</v>
+        <v>63.926902445871541</v>
       </c>
       <c r="CK34" s="8">
         <f t="shared" si="7"/>
-        <v>64.278974004146662</v>
+        <v>64.221442987161737</v>
       </c>
       <c r="CL34" s="8">
         <f t="shared" si="7"/>
-        <v>64.096506326438558</v>
+        <v>64.038975309453633</v>
       </c>
       <c r="CM34" s="8">
         <f t="shared" si="7"/>
-        <v>64.338923802161375</v>
+        <v>64.28139278517645</v>
       </c>
       <c r="CN34" s="8">
         <f t="shared" si="7"/>
-        <v>64.405252606536251</v>
+        <v>64.347721589551327</v>
       </c>
       <c r="CO34" s="8">
         <f t="shared" si="7"/>
-        <v>64.137470612031834</v>
+        <v>64.079939595046909</v>
       </c>
       <c r="CP34" s="8">
         <f t="shared" si="7"/>
-        <v>64.193208123230889</v>
+        <v>64.135677106245964</v>
       </c>
       <c r="CQ34" s="8">
         <f t="shared" si="7"/>
-        <v>64.096794105720448</v>
+        <v>64.039263088735524</v>
       </c>
       <c r="CR34" s="8">
         <f t="shared" si="7"/>
-        <v>64.350573140840254</v>
+        <v>64.293042123855329</v>
       </c>
       <c r="CS34" s="8">
         <f t="shared" si="7"/>
-        <v>64.407241330388516</v>
+        <v>64.349710313403591</v>
       </c>
       <c r="CT34" s="8">
         <f t="shared" si="7"/>
-        <v>64.382052798831694</v>
+        <v>64.324521781846769</v>
       </c>
       <c r="CU34" s="8">
         <f t="shared" si="7"/>
-        <v>64.65150777094442</v>
+        <v>64.593976753959495</v>
       </c>
       <c r="CV34" s="8">
         <f t="shared" si="7"/>
-        <v>64.090756159873436</v>
+        <v>64.033225142888512</v>
       </c>
       <c r="CW34" s="8">
         <f t="shared" si="7"/>
-        <v>64.413950672803495</v>
+        <v>64.35641965581857</v>
       </c>
       <c r="CX34" s="8">
         <f t="shared" si="7"/>
-        <v>64.601226242670066</v>
+        <v>64.543695225685141</v>
       </c>
       <c r="CY34" s="9">
         <f t="shared" si="7"/>
-        <v>64.558156969485154</v>
+        <v>64.500625952500229</v>
       </c>
     </row>
     <row r="35" spans="1:103" x14ac:dyDescent="0.2">
@@ -11475,7 +12629,7 @@
       </c>
       <c r="N35" s="7" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O35" s="7" t="b">
         <f t="shared" si="8"/>
@@ -11503,7 +12657,7 @@
       </c>
       <c r="U35" s="7" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V35" s="7" t="b">
         <f t="shared" si="8"/>
@@ -11563,7 +12717,7 @@
       </c>
       <c r="AJ35" s="7" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK35" s="7" t="b">
         <f t="shared" si="8"/>
@@ -11647,7 +12801,7 @@
       </c>
       <c r="BE35" s="7" t="b">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF35" s="7" t="b">
         <f t="shared" si="8"/>
@@ -11707,7 +12861,7 @@
       </c>
       <c r="BT35" s="7" t="b">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU35" s="7" t="b">
         <f t="shared" si="9"/>
@@ -12285,7 +13439,7 @@
       </c>
       <c r="N37" s="11" t="str">
         <f t="shared" si="12"/>
-        <v>R</v>
+        <v>DR</v>
       </c>
       <c r="O37" s="11" t="str">
         <f t="shared" si="12"/>
@@ -12301,7 +13455,7 @@
       </c>
       <c r="R37" s="11" t="str">
         <f t="shared" si="12"/>
-        <v>R</v>
+        <v>DR</v>
       </c>
       <c r="S37" s="11" t="str">
         <f t="shared" si="12"/>
@@ -12313,11 +13467,11 @@
       </c>
       <c r="U37" s="11" t="str">
         <f t="shared" si="12"/>
-        <v>R</v>
+        <v>DR</v>
       </c>
       <c r="V37" s="11" t="str">
         <f t="shared" si="12"/>
-        <v>R</v>
+        <v>DR</v>
       </c>
       <c r="W37" s="11" t="str">
         <f t="shared" si="12"/>
@@ -12349,7 +13503,7 @@
       </c>
       <c r="AD37" s="11" t="str">
         <f t="shared" si="12"/>
-        <v>R</v>
+        <v>DR</v>
       </c>
       <c r="AE37" s="11" t="str">
         <f t="shared" si="12"/>
@@ -12373,7 +13527,7 @@
       </c>
       <c r="AJ37" s="11" t="str">
         <f t="shared" si="12"/>
-        <v>R</v>
+        <v>DR</v>
       </c>
       <c r="AK37" s="11" t="str">
         <f t="shared" si="12"/>
@@ -12457,7 +13611,7 @@
       </c>
       <c r="BE37" s="11" t="str">
         <f t="shared" si="12"/>
-        <v>R</v>
+        <v>DR</v>
       </c>
       <c r="BF37" s="11" t="str">
         <f t="shared" si="12"/>
@@ -12517,7 +13671,7 @@
       </c>
       <c r="BT37" s="11" t="str">
         <f t="shared" si="13"/>
-        <v>R</v>
+        <v>DR</v>
       </c>
       <c r="BU37" s="11" t="str">
         <f t="shared" si="13"/>
@@ -12581,7 +13735,7 @@
       </c>
       <c r="CJ37" s="11" t="str">
         <f t="shared" si="13"/>
-        <v>R</v>
+        <v>DR</v>
       </c>
       <c r="CK37" s="11" t="str">
         <f t="shared" si="13"/>
@@ -12862,13 +14016,18 @@
       </c>
       <c r="C41" s="16">
         <f>COUNTIF(D35:CY35,"=FALSE")</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
+      <c r="G41" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" s="16">
+        <f>COUNTIF(D37:CY37, "=DR")</f>
+        <v>98</v>
+      </c>
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
@@ -12972,8 +14131,13 @@
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="G42" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" s="16">
+        <f>H41/100</f>
+        <v>0.98</v>
+      </c>
       <c r="I42" s="16"/>
       <c r="J42" s="16"/>
       <c r="K42" s="16"/>
@@ -16862,10 +18026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:CZ49"/>
+  <dimension ref="A1:CZ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H49" sqref="G36:H49"/>
+    <sheetView tabSelected="1" topLeftCell="Q23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16878,6 +18042,8 @@
     <col min="6" max="6" width="5.140625" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.85546875" customWidth="1"/>
     <col min="19" max="19" width="11.140625" customWidth="1"/>
   </cols>
@@ -16907,6 +18073,10 @@
       <c r="C2">
         <v>66.5</v>
       </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>1.7999999999999972</v>
+      </c>
       <c r="E2">
         <v>62.723180851811776</v>
       </c>
@@ -17218,6 +18388,10 @@
       <c r="C3">
         <v>66</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D31" si="0">C3-B3</f>
+        <v>1.0999999999999943</v>
+      </c>
       <c r="E3">
         <v>64.541692770639202</v>
       </c>
@@ -17529,6 +18703,10 @@
       <c r="C4">
         <v>67.3</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="E4">
         <v>64.315230863634497</v>
       </c>
@@ -17840,6 +19018,10 @@
       <c r="C5">
         <v>66.8</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1.7999999999999972</v>
+      </c>
       <c r="E5">
         <v>63.579713403363712</v>
       </c>
@@ -18151,6 +19333,10 @@
       <c r="C6">
         <v>66.5</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1.9000000000000057</v>
+      </c>
       <c r="E6">
         <v>64.730171905161114</v>
       </c>
@@ -18462,6 +19648,10 @@
       <c r="C7">
         <v>66.099999999999994</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999972</v>
+      </c>
       <c r="E7">
         <v>64.345689841196872</v>
       </c>
@@ -18773,6 +19963,10 @@
       <c r="C8">
         <v>66.900000000000006</v>
       </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="E8">
         <v>62.563580447807908</v>
       </c>
@@ -19084,6 +20278,10 @@
       <c r="C9">
         <v>66.3</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000028</v>
+      </c>
       <c r="E9">
         <v>63.768883753858972</v>
       </c>
@@ -19395,6 +20593,10 @@
       <c r="C10">
         <v>66.900000000000006</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="E10">
         <v>63.943935335977585</v>
       </c>
@@ -19706,6 +20908,10 @@
       <c r="C11">
         <v>67.099999999999994</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999886</v>
+      </c>
       <c r="E11">
         <v>63.887347712501651</v>
       </c>
@@ -20017,6 +21223,10 @@
       <c r="C12">
         <v>66.7</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
       <c r="E12">
         <v>64.069325096774264</v>
       </c>
@@ -20328,6 +21538,10 @@
       <c r="C13">
         <v>66.2</v>
       </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1.4000000000000057</v>
+      </c>
       <c r="E13">
         <v>63.649025994585827</v>
       </c>
@@ -20639,6 +21853,10 @@
       <c r="C14">
         <v>69.099999999999994</v>
       </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>9.9999999999994316E-2</v>
+      </c>
       <c r="E14">
         <v>64.727677615941502</v>
       </c>
@@ -20950,6 +22168,10 @@
       <c r="C15">
         <v>67.099999999999994</v>
       </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.89999999999999147</v>
+      </c>
       <c r="E15">
         <v>63.837609720998444</v>
       </c>
@@ -21261,6 +22483,10 @@
       <c r="C16">
         <v>66.900000000000006</v>
       </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1.6000000000000085</v>
+      </c>
       <c r="E16">
         <v>63.198221303231549</v>
       </c>
@@ -21572,6 +22798,10 @@
       <c r="C17">
         <v>66.900000000000006</v>
       </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000114</v>
+      </c>
       <c r="E17">
         <v>64.655286385153886</v>
       </c>
@@ -21883,6 +23113,10 @@
       <c r="C18">
         <v>66.3</v>
       </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999943</v>
+      </c>
       <c r="E18">
         <v>65.849439286161214</v>
       </c>
@@ -22194,6 +23428,10 @@
       <c r="C19">
         <v>66.900000000000006</v>
       </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000028</v>
+      </c>
       <c r="E19">
         <v>63.478484369319631</v>
       </c>
@@ -22505,6 +23743,10 @@
       <c r="C20">
         <v>67.3</v>
       </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999972</v>
+      </c>
       <c r="E20">
         <v>65.867074388428591</v>
       </c>
@@ -22816,6 +24058,10 @@
       <c r="C21">
         <v>66.599999999999994</v>
       </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999943</v>
+      </c>
       <c r="E21">
         <v>63.650572135578841</v>
       </c>
@@ -23127,6 +24373,10 @@
       <c r="C22">
         <v>66.8</v>
       </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>2.2999999999999972</v>
+      </c>
       <c r="E22">
         <v>64.989418822427979</v>
       </c>
@@ -23438,6 +24688,10 @@
       <c r="C23">
         <v>66.5</v>
       </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
       <c r="E23">
         <v>65.064734078681795</v>
       </c>
@@ -23749,6 +25003,10 @@
       <c r="C24">
         <v>66.599999999999994</v>
       </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999972</v>
+      </c>
       <c r="E24">
         <v>65.172402335214429</v>
       </c>
@@ -24060,6 +25318,10 @@
       <c r="C25">
         <v>68.099999999999994</v>
       </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0.69999999999998863</v>
+      </c>
       <c r="E25">
         <v>65.444404915673658</v>
       </c>
@@ -24371,6 +25633,10 @@
       <c r="C26">
         <v>66.7</v>
       </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>1.9000000000000057</v>
+      </c>
       <c r="E26">
         <v>63.106507857504766</v>
       </c>
@@ -24682,6 +25948,10 @@
       <c r="C27">
         <v>66.900000000000006</v>
       </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000114</v>
+      </c>
       <c r="E27">
         <v>64.284264842775883</v>
       </c>
@@ -24993,6 +26263,10 @@
       <c r="C28">
         <v>66.7</v>
       </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>1.9000000000000057</v>
+      </c>
       <c r="E28">
         <v>65.188991518574767</v>
       </c>
@@ -25304,6 +26578,10 @@
       <c r="C29">
         <v>66.900000000000006</v>
       </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0.80000000000001137</v>
+      </c>
       <c r="E29">
         <v>64.392205947719049</v>
       </c>
@@ -25615,6 +26893,10 @@
       <c r="C30">
         <v>66.5</v>
       </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999943</v>
+      </c>
       <c r="E30">
         <v>63.972495743350009</v>
       </c>
@@ -25926,6 +27208,10 @@
       <c r="C31">
         <v>66.599999999999994</v>
       </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>1.8999999999999915</v>
+      </c>
       <c r="E31">
         <v>63.765268512419425</v>
       </c>
@@ -26227,8 +27513,8 @@
         <v>64.343011379300151</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
         <v>11</v>
       </c>
@@ -26242,7 +27528,7 @@
       </c>
       <c r="H34" s="23"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="D35" s="21"/>
@@ -26250,7 +27536,7 @@
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>17</v>
       </c>
@@ -26269,8 +27555,15 @@
       <c r="H36" s="21">
         <v>66.823333333333338</v>
       </c>
+      <c r="J36">
+        <f>TDIST(3.019553976, 29, 1)</f>
+        <v>2.6185002209360825E-3</v>
+      </c>
+      <c r="L36" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>18</v>
       </c>
@@ -26290,7 +27583,7 @@
         <v>0.1083505733408688</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>19</v>
       </c>
@@ -26309,8 +27602,18 @@
       <c r="H38" s="21">
         <v>66.75</v>
       </c>
+      <c r="L38" s="24"/>
+      <c r="M38" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="N38" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="P38" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>20</v>
       </c>
@@ -26329,8 +27632,21 @@
       <c r="H39" s="21">
         <v>66.900000000000006</v>
       </c>
+      <c r="L39" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M39" s="21">
+        <v>65.089999999999989</v>
+      </c>
+      <c r="N39" s="21">
+        <v>65.273333333333341</v>
+      </c>
+      <c r="T39" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="U39" s="23"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
         <v>21</v>
       </c>
@@ -26349,8 +27665,26 @@
       <c r="H40" s="21">
         <v>0.59346053137411725</v>
       </c>
+      <c r="L40" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="M40" s="21">
+        <v>3.9092068965517264</v>
+      </c>
+      <c r="N40" s="21">
+        <v>0.84271264367816123</v>
+      </c>
+      <c r="P40" s="24"/>
+      <c r="Q40" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="R40" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="T40" s="21"/>
+      <c r="U40" s="21"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
         <v>22</v>
       </c>
@@ -26369,8 +27703,36 @@
       <c r="H41" s="21">
         <v>0.35219540229884966</v>
       </c>
+      <c r="J41">
+        <f>_xlfn.T.DIST(0.025,29,1)</f>
+        <v>0.50988689907209583</v>
+      </c>
+      <c r="L41" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="M41" s="21">
+        <v>30</v>
+      </c>
+      <c r="N41" s="21">
+        <v>30</v>
+      </c>
+      <c r="P41" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q41" s="21">
+        <v>65.273333333333341</v>
+      </c>
+      <c r="R41" s="21">
+        <v>66.823333333333338</v>
+      </c>
+      <c r="T41" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="U41" s="21">
+        <v>1.5499999999999996</v>
+      </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
         <v>23</v>
       </c>
@@ -26389,8 +27751,30 @@
       <c r="H42" s="21">
         <v>7.1694081329165087</v>
       </c>
+      <c r="L42" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="M42" s="21">
+        <v>0</v>
+      </c>
+      <c r="N42" s="21"/>
+      <c r="P42" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q42" s="21">
+        <v>0.84271264367816123</v>
+      </c>
+      <c r="R42" s="21">
+        <v>0.35219540229884966</v>
+      </c>
+      <c r="T42" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="U42" s="21">
+        <v>9.169539779624461E-2</v>
+      </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
         <v>24</v>
       </c>
@@ -26409,8 +27793,30 @@
       <c r="H43" s="21">
         <v>2.2101763893616382</v>
       </c>
+      <c r="L43" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="M43" s="21">
+        <v>41</v>
+      </c>
+      <c r="N43" s="21"/>
+      <c r="P43" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q43" s="21">
+        <v>30</v>
+      </c>
+      <c r="R43" s="21">
+        <v>30</v>
+      </c>
+      <c r="T43" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="U43" s="21">
+        <v>1.6000000000000014</v>
+      </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
         <v>25</v>
       </c>
@@ -26429,8 +27835,28 @@
       <c r="H44" s="21">
         <v>3.0999999999999943</v>
       </c>
+      <c r="L44" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="M44" s="21">
+        <v>-0.46064623178833752</v>
+      </c>
+      <c r="N44" s="21"/>
+      <c r="P44" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q44" s="21">
+        <v>0.86516025241507288</v>
+      </c>
+      <c r="R44" s="21"/>
+      <c r="T44" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="U44" s="21">
+        <v>2</v>
+      </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="s">
         <v>26</v>
       </c>
@@ -26449,8 +27875,28 @@
       <c r="H45" s="21">
         <v>66</v>
       </c>
+      <c r="L45" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="M45" s="21">
+        <v>0.32374327046157053</v>
+      </c>
+      <c r="N45" s="21"/>
+      <c r="P45" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q45" s="21">
+        <v>0</v>
+      </c>
+      <c r="R45" s="21"/>
+      <c r="T45" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="U45" s="21">
+        <v>0.50223637792412668</v>
+      </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
         <v>27</v>
       </c>
@@ -26469,8 +27915,28 @@
       <c r="H46" s="21">
         <v>69.099999999999994</v>
       </c>
+      <c r="L46" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="M46" s="21">
+        <v>1.6828780021327077</v>
+      </c>
+      <c r="N46" s="21"/>
+      <c r="P46" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q46" s="21">
+        <v>29</v>
+      </c>
+      <c r="R46" s="21"/>
+      <c r="T46" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="U46" s="21">
+        <v>0.25224137931034624</v>
+      </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>28</v>
       </c>
@@ -26489,8 +27955,28 @@
       <c r="H47" s="21">
         <v>2004.7</v>
       </c>
+      <c r="L47" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="M47" s="21">
+        <v>0.64748654092314106</v>
+      </c>
+      <c r="N47" s="21"/>
+      <c r="P47" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q47" s="21">
+        <v>-16.903792744803162</v>
+      </c>
+      <c r="R47" s="21"/>
+      <c r="T47" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="U47" s="21">
+        <v>0.94210438287651455</v>
+      </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
         <v>29</v>
       </c>
@@ -26509,8 +27995,28 @@
       <c r="H48" s="21">
         <v>30</v>
       </c>
+      <c r="L48" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="M48" s="22">
+        <v>2.0195409704413767</v>
+      </c>
+      <c r="N48" s="22"/>
+      <c r="P48" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q48" s="21">
+        <v>7.4139717237406197E-17</v>
+      </c>
+      <c r="R48" s="21"/>
+      <c r="T48" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="U48" s="21">
+        <v>-0.92040235491693501</v>
+      </c>
     </row>
-    <row r="49" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>30</v>
       </c>
@@ -26528,6 +28034,73 @@
       </c>
       <c r="H49" s="22">
         <v>0.22160180433881832</v>
+      </c>
+      <c r="P49" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q49" s="21">
+        <v>1.6991270265334986</v>
+      </c>
+      <c r="R49" s="21"/>
+      <c r="T49" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="U49" s="21">
+        <v>2.2000000000000028</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="P50" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q50" s="21">
+        <v>1.4827943447481239E-16</v>
+      </c>
+      <c r="R50" s="21"/>
+      <c r="T50" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="U50" s="21">
+        <v>9.9999999999994316E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P51" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q51" s="22">
+        <v>2.0452296421327048</v>
+      </c>
+      <c r="R51" s="22"/>
+      <c r="T51" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="U51" s="21">
+        <v>2.2999999999999972</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T52" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="U52" s="21">
+        <v>46.499999999999986</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T53" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="U53" s="21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T54" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="U54" s="22">
+        <v>0.18753814562002924</v>
       </c>
     </row>
   </sheetData>
@@ -26535,5 +28108,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>